<commit_message>
Added in code to run a cpuTest
</commit_message>
<xml_diff>
--- a/CollisionChart.xlsx
+++ b/CollisionChart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NumberCollisionsData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Number of Records</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Best Performance</t>
+  </si>
+  <si>
+    <t>CPU Time (msec)</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +1594,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B2:E14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2234,12 +2237,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2248,7 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated probe functions to use pseudo random instead of double hashing as per the project requirements3
</commit_message>
<xml_diff>
--- a/CollisionChart.xlsx
+++ b/CollisionChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwasf\Dropbox\School\CS3100\Projects\Project4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian\Dropbox\School\CS3100\Projects\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,12 @@
     <sheet name="NumberCollisionsData" sheetId="1" r:id="rId1"/>
     <sheet name="CPUUsageData" sheetId="2" r:id="rId2"/>
     <sheet name="PivotChartNumberCollisions" sheetId="3" r:id="rId3"/>
+    <sheet name="PivotChartCPUUsageData" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="10" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Number of Records</t>
   </si>
@@ -59,6 +61,12 @@
   </si>
   <si>
     <t>CPU Time (msec)</t>
+  </si>
+  <si>
+    <t>Number of Records (% of total)</t>
+  </si>
+  <si>
+    <t>Sum of CPU Time (msec)</t>
   </si>
 </sst>
 </file>
@@ -94,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -107,11 +115,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -205,9 +228,34 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8987690706079861E-2"/>
+          <c:y val="0.14249781277340332"/>
+          <c:w val="0.74551826966077961"/>
+          <c:h val="0.57697980460775733"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -246,34 +294,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>800</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1000</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -288,34 +336,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>84</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>115</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>191</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>298</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>581</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2856</c:v>
+                  <c:v>2125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,34 +410,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>800</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1000</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -404,34 +452,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>282</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>308</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>343</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>515</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2626</c:v>
+                  <c:v>2893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,34 +526,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>800</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1000</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -886,6 +934,511 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[CollisionChart.xlsx]PivotChartCPUUsageData!PivotTable2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPU</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Time</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChartCPUUsageData!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChartCPUUsageData!$A$4:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChartCPUUsageData!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FF3-4B2F-BA92-9C275B986EF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="352212632"/>
+        <c:axId val="352214272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="352212632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of insertions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352214272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="352214272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (msec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352212632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -926,7 +1479,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1483,35 +2592,108 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94397855-3903-4420-9250-1C7DA8678650}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="kewlstore" refreshedDate="42845.47944664352" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ian" refreshedDate="42845.820728240738" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="4">
-    <cacheField name="Number of Records" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1000" count="11">
+    <cacheField name="Number of Records (% of total)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.99" count="11">
         <n v="0"/>
-        <n v="100"/>
-        <n v="200"/>
-        <n v="300"/>
-        <n v="400"/>
-        <n v="500"/>
-        <n v="600"/>
-        <n v="700"/>
-        <n v="800"/>
-        <n v="900"/>
-        <n v="1000"/>
+        <n v="0.1"/>
+        <n v="0.2"/>
+        <n v="0.3"/>
+        <n v="0.4"/>
+        <n v="0.5"/>
+        <n v="0.6"/>
+        <n v="0.7"/>
+        <n v="0.8"/>
+        <n v="0.9"/>
+        <n v="0.99"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Number of Collisions (Sequential)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2856"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2125"/>
     </cacheField>
     <cacheField name="Number Of Collisions (Randomized)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2626"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2893"/>
     </cacheField>
     <cacheField name="Number Of Collisions (Best)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="112.111"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ian" refreshedDate="42845.837738657407" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="10">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B2:C12" sheet="CPUUsageData"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Number of Records" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="1000" count="10">
+        <n v="900"/>
+        <n v="1000"/>
+        <n v="800"/>
+        <n v="700"/>
+        <n v="400"/>
+        <n v="600"/>
+        <n v="300"/>
+        <n v="500"/>
+        <n v="200"/>
+        <n v="100"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="CPU Time (msec)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6" maxValue="29"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1532,73 +2714,118 @@
   </r>
   <r>
     <x v="1"/>
-    <n v="6"/>
-    <n v="10"/>
+    <n v="0"/>
+    <n v="1"/>
     <n v="1.109"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="12"/>
-    <n v="26"/>
+    <n v="0"/>
+    <n v="6"/>
     <n v="1.2470000000000001"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="25"/>
-    <n v="35"/>
+    <n v="0"/>
+    <n v="13"/>
     <n v="1.423"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="55"/>
-    <n v="61"/>
+    <n v="0"/>
+    <n v="19"/>
     <n v="1.6559999999999999"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="84"/>
-    <n v="93"/>
+    <n v="7"/>
+    <n v="19"/>
     <n v="1.982"/>
   </r>
   <r>
     <x v="6"/>
-    <n v="115"/>
-    <n v="282"/>
+    <n v="52"/>
+    <n v="209"/>
     <n v="2.4689999999999999"/>
   </r>
   <r>
     <x v="7"/>
-    <n v="191"/>
-    <n v="308"/>
+    <n v="75"/>
+    <n v="344"/>
     <n v="3.2650000000000001"/>
   </r>
   <r>
     <x v="8"/>
-    <n v="298"/>
-    <n v="343"/>
+    <n v="276"/>
+    <n v="476"/>
     <n v="4.827"/>
   </r>
   <r>
     <x v="9"/>
-    <n v="581"/>
-    <n v="515"/>
+    <n v="260"/>
+    <n v="657"/>
     <n v="9.2569999999999997"/>
   </r>
   <r>
     <x v="10"/>
-    <n v="2856"/>
-    <n v="2626"/>
+    <n v="2125"/>
+    <n v="2893"/>
     <n v="112.111"/>
   </r>
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+  <r>
+    <x v="0"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="6"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B2:E14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1610,7 +2837,6 @@
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
-        <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
@@ -1715,14 +2941,113 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="9"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of CPU Time (msec)" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:D12"/>
   <tableColumns count="4">
+    <tableColumn id="1" name="Number of Records (% of total)" dataDxfId="7"/>
+    <tableColumn id="2" name="Number of Collisions (Sequential)" dataDxfId="6"/>
+    <tableColumn id="3" name="Number Of Collisions (Randomized)" dataDxfId="5"/>
+    <tableColumn id="4" name="Number Of Collisions (Best)" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B2:C12"/>
+  <sortState ref="B3:C12">
+    <sortCondition ref="B2:B12"/>
+  </sortState>
+  <tableColumns count="2">
     <tableColumn id="1" name="Number of Records" dataDxfId="3"/>
-    <tableColumn id="2" name="Number of Collisions (Sequential)" dataDxfId="2"/>
-    <tableColumn id="3" name="Number Of Collisions (Randomized)" dataDxfId="1"/>
-    <tableColumn id="4" name="Number Of Collisions (Best)" dataDxfId="0"/>
+    <tableColumn id="2" name="CPU Time (msec)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2028,12 +3353,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
@@ -2045,7 +3370,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -2075,13 +3400,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="B3" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>1.109</v>
@@ -2090,13 +3415,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="B4" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>1.2470000000000001</v>
@@ -2105,13 +3430,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="B5" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>1.423</v>
@@ -2120,13 +3445,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="B6" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>1.6559999999999999</v>
@@ -2135,13 +3460,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="B7" s="1">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>1.982</v>
@@ -2150,13 +3475,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>600</v>
+        <v>0.6</v>
       </c>
       <c r="B8" s="1">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1">
-        <v>282</v>
+        <v>209</v>
       </c>
       <c r="D8" s="1">
         <v>2.4689999999999999</v>
@@ -2165,13 +3490,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>700</v>
+        <v>0.7</v>
       </c>
       <c r="B9" s="1">
-        <v>191</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="D9" s="1">
         <v>3.2650000000000001</v>
@@ -2180,13 +3505,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>800</v>
+        <v>0.8</v>
       </c>
       <c r="B10" s="1">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="C10" s="1">
-        <v>343</v>
+        <v>476</v>
       </c>
       <c r="D10" s="1">
         <v>4.827</v>
@@ -2195,13 +3520,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>900</v>
+        <v>0.9</v>
       </c>
       <c r="B11" s="1">
-        <v>581</v>
+        <v>260</v>
       </c>
       <c r="C11" s="1">
-        <v>515</v>
+        <v>657</v>
       </c>
       <c r="D11" s="1">
         <v>9.2569999999999997</v>
@@ -2210,13 +3535,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1000</v>
+        <v>0.99</v>
       </c>
       <c r="B12" s="1">
-        <v>2856</v>
+        <v>2125</v>
       </c>
       <c r="C12" s="1">
-        <v>2626</v>
+        <v>2893</v>
       </c>
       <c r="D12" s="1">
         <v>112.111</v>
@@ -2237,28 +3562,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>100</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>200</v>
+      </c>
+      <c r="C4" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>300</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>400</v>
+      </c>
+      <c r="C6" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>500</v>
+      </c>
+      <c r="C7" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>600</v>
+      </c>
+      <c r="C8" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>700</v>
+      </c>
+      <c r="C9" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>800</v>
+      </c>
+      <c r="C10" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>900</v>
+      </c>
+      <c r="C11" s="6">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="6">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2266,199 +3678,315 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E14"/>
   <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.2470000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.423</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.982</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2">
+        <v>209</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.4689999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2">
+        <v>344</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3.2650000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>276</v>
+      </c>
+      <c r="D11" s="2">
+        <v>476</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.827</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>260</v>
+      </c>
+      <c r="D12" s="2">
+        <v>657</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9.2569999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2125</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2893</v>
+      </c>
+      <c r="E13" s="2">
+        <v>112.111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2795</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4637</v>
+      </c>
+      <c r="E14" s="2">
+        <v>139.346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B14"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
-        <v>100</v>
-      </c>
-      <c r="C4" s="2">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.109</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>200</v>
       </c>
-      <c r="C5" s="2">
+      <c r="B5" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>300</v>
+      </c>
+      <c r="B6" s="2">
         <v>12</v>
       </c>
-      <c r="D5" s="2">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.2470000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>300</v>
-      </c>
-      <c r="C6" s="2">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.423</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>400</v>
       </c>
-      <c r="C7" s="2">
-        <v>55</v>
-      </c>
-      <c r="D7" s="2">
-        <v>61</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.6559999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="B7" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>500</v>
       </c>
-      <c r="C8" s="2">
-        <v>84</v>
-      </c>
-      <c r="D8" s="2">
-        <v>93</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.982</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+      <c r="B8" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>600</v>
       </c>
-      <c r="C9" s="2">
-        <v>115</v>
-      </c>
-      <c r="D9" s="2">
-        <v>282</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2.4689999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+      <c r="B9" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>700</v>
       </c>
-      <c r="C10" s="2">
-        <v>191</v>
-      </c>
-      <c r="D10" s="2">
-        <v>308</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3.2650000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
+      <c r="B10" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>800</v>
       </c>
-      <c r="C11" s="2">
-        <v>298</v>
-      </c>
-      <c r="D11" s="2">
-        <v>343</v>
-      </c>
-      <c r="E11" s="2">
-        <v>4.827</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+      <c r="B11" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>900</v>
       </c>
-      <c r="C12" s="2">
-        <v>581</v>
-      </c>
-      <c r="D12" s="2">
-        <v>515</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9.2569999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
+      <c r="B12" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="C13" s="2">
-        <v>2856</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2626</v>
-      </c>
-      <c r="E13" s="2">
-        <v>112.111</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B13" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
-        <v>4223</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4299</v>
-      </c>
-      <c r="E14" s="2">
-        <v>139.346</v>
+      <c r="B14" s="2">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated documentation for hash table, and finalized AnalysisReport and CollisionChart data.
</commit_message>
<xml_diff>
--- a/CollisionChart.xlsx
+++ b/CollisionChart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian\Dropbox\School\CS3100\Projects\Project4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwasf\Dropbox\School\CS3100\Projects\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NumberCollisionsData" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
-    <pivotCache cacheId="10" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -231,6 +231,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2821,7 +2824,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="B2:E14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -2942,7 +2945,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -3040,14 +3043,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C12" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="B2:C12"/>
   <sortState ref="B3:C12">
     <sortCondition ref="B2:B12"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Number of Records" dataDxfId="3"/>
-    <tableColumn id="2" name="CPU Time (msec)" dataDxfId="2"/>
+    <tableColumn id="1" name="Number of Records" dataDxfId="1"/>
+    <tableColumn id="2" name="CPU Time (msec)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3353,7 +3356,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,7 +3567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3678,8 +3681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>